<commit_message>
Finish refactoring after pandas switch
</commit_message>
<xml_diff>
--- a/data/example.xlsx
+++ b/data/example.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+  <si>
+    <t xml:space="preserve">IOChannels</t>
+  </si>
   <si>
     <t xml:space="preserve">delete</t>
   </si>
@@ -197,7 +200,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -213,83 +216,86 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -300,7 +306,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>13</v>
@@ -326,7 +332,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>26</v>
@@ -352,7 +358,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>39</v>
@@ -378,7 +384,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>52</v>
@@ -404,7 +410,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>65</v>
@@ -430,7 +436,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>78</v>
@@ -456,7 +462,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>91</v>
@@ -482,7 +488,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>104</v>
@@ -508,7 +514,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>130</v>
@@ -534,7 +540,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>151</v>
@@ -555,11 +561,11 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:G4" type="list">
-      <formula1>#REF!</formula1>
+      <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A5:G5" type="list">
-      <formula1>#REF!</formula1>
+      <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>